<commit_message>
Completed full scenario of StockIn
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/SmokeTestData.xlsx
+++ b/src/test/resources/testdata/SmokeTestData.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Optimnet\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29D63CF-2846-4622-ACF3-1DBC1381C71F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38ACE894-531E-45D4-AB83-6560614125F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="logindata" sheetId="5" r:id="rId1"/>
     <sheet name="newStockContactLens" sheetId="8" r:id="rId2"/>
-    <sheet name="newStockGeneral" sheetId="1" r:id="rId3"/>
-    <sheet name="contactLensEntry" sheetId="6" r:id="rId4"/>
-    <sheet name="newStockLens" sheetId="7" r:id="rId5"/>
-    <sheet name="stockTransfer" sheetId="2" r:id="rId6"/>
-    <sheet name="order" sheetId="3" r:id="rId7"/>
-    <sheet name="Bill" sheetId="4" r:id="rId8"/>
+    <sheet name="newLensStock" sheetId="9" r:id="rId3"/>
+    <sheet name="newStockGeneral" sheetId="1" r:id="rId4"/>
+    <sheet name="contactLensEntry" sheetId="6" r:id="rId5"/>
+    <sheet name="newStockLens" sheetId="7" r:id="rId6"/>
+    <sheet name="stockTransfer" sheetId="2" r:id="rId7"/>
+    <sheet name="order" sheetId="3" r:id="rId8"/>
+    <sheet name="Bill" sheetId="4" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="88">
   <si>
     <t>Category</t>
   </si>
@@ -260,13 +261,49 @@
   </si>
   <si>
     <t>DAILY</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>material</t>
+  </si>
+  <si>
+    <t>coat</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>qty</t>
+  </si>
+  <si>
+    <t>rate</t>
+  </si>
+  <si>
+    <t>sprice</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>MAHADEV OPTICALS</t>
+  </si>
+  <si>
+    <t>1.67RI</t>
+  </si>
+  <si>
+    <t>CLEAR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,8 +325,21 @@
       <name val="Arial Black"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,6 +370,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -333,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -360,6 +416,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -685,7 +750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D8BCD0-864F-40B4-BED8-3AEF908039CF}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -778,6 +843,116 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D19426E-73DF-4AE0-8E9A-25B7580B05F2}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="11">
+        <v>5</v>
+      </c>
+      <c r="I2" s="11">
+        <v>2500</v>
+      </c>
+      <c r="J2" s="11">
+        <v>5000</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="K2:N2" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -890,7 +1065,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAAD79CC-BE19-4BFE-A044-986D4365C117}">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -970,12 +1145,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17573C3B-811A-47F6-A92B-E95BE5705710}">
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A2" sqref="A2:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1166,7 +1341,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0283403E-6E64-4CF1-A9BF-B9189799B7C3}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -1251,7 +1426,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13A83F9-CCC4-49B3-92E8-F39F19047387}">
   <dimension ref="A1:L5"/>
   <sheetViews>
@@ -1364,7 +1539,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{076A733D-3CC2-4378-9E0F-6B4D2E50AB5C}">
   <dimension ref="A1:B3"/>
   <sheetViews>

</xml_diff>